<commit_message>
update info cost cloud provider
</commit_message>
<xml_diff>
--- a/macro_backlog&estimation_couts.xlsx
+++ b/macro_backlog&estimation_couts.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/268a6ad7fabc2896/Documents/OPENCLASSROOMS/Projet 13 Passez votre systeme IA du POC au MVP et réalisez votre portfolio de Data Engineer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="11_F25DC773A252ABDACC104856F19A601C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AEEE54A-8335-411A-ABB7-5B908A6E1199}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="11_F25DC773A252ABDACC104856F19A601C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EAF3078-5440-465B-8141-C6A8A801BCC3}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="macro_backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Coûts BUILD (développement init" sheetId="2" r:id="rId2"/>
     <sheet name="Coûts OPEX (exploitation)" sheetId="3" r:id="rId3"/>
-    <sheet name="Optimisation budgétaire" sheetId="4" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="5" r:id="rId4"/>
+    <sheet name="Optimisation budgétaire" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="168">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -261,9 +262,6 @@
     <t>Modélisation et mise en place des métadonnées</t>
   </si>
   <si>
-    <t>Faible à moyenne</t>
-  </si>
-  <si>
     <t>Vectorisation NLP</t>
   </si>
   <si>
@@ -297,66 +295,30 @@
     <t>Documentation technique &amp; projet</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Impact selon charge utilisateur</t>
-  </si>
-  <si>
     <t>Hébergement cloud</t>
   </si>
   <si>
-    <t>Exécution API, RAG, UI (conteneurs)</t>
-  </si>
-  <si>
     <t>Récurrent</t>
   </si>
   <si>
     <t>Moyen</t>
   </si>
   <si>
-    <t>Métadonnées événements</t>
-  </si>
-  <si>
     <t>Stockage vectoriel</t>
   </si>
   <si>
-    <t>Index embeddings FAISS</t>
-  </si>
-  <si>
-    <t>Faible à moyen</t>
-  </si>
-  <si>
     <t>Appels NLP / LLM</t>
   </si>
   <si>
-    <t>Embeddings + génération RAG</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Élevé</t>
-  </si>
-  <si>
     <t>Réseau</t>
   </si>
   <si>
-    <t>Appels API, flux entrants/sortants</t>
-  </si>
-  <si>
     <t>Monitoring &amp; logs</t>
   </si>
   <si>
-    <t>Collecte métriques et erreurs</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Correctifs et ajustements</t>
-  </si>
-  <si>
     <t>Levier</t>
   </si>
   <si>
@@ -412,12 +374,174 @@
   </si>
   <si>
     <t>Pérennité</t>
+  </si>
+  <si>
+    <t>Coût</t>
+  </si>
+  <si>
+    <t>6 joiurs</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>33 jours</t>
+  </si>
+  <si>
+    <t>Détail du périmètre couvert</t>
+  </si>
+  <si>
+    <t>Hypothèses retenues</t>
+  </si>
+  <si>
+    <t>Type de coût</t>
+  </si>
+  <si>
+    <t>Hébergement de l’API Backend, du moteur RAG et de l’interface utilisateur via des conteneurs (Azure App Service / Container Apps)</t>
+  </si>
+  <si>
+    <t>Charge faible à modérée (phase MVP, trafic limité)</t>
+  </si>
+  <si>
+    <t>Base de données pour les métadonnées structurées des événements (dates, lieux, catégories, descriptions courtes)</t>
+  </si>
+  <si>
+    <t>Volume &lt; 1 Go, faible nombre d’écritures</t>
+  </si>
+  <si>
+    <t>Stockage local de l’index FAISS et des embeddings vectoriels</t>
+  </si>
+  <si>
+    <t>FAISS embarqué, stockage disque inclus dans l’hébergement</t>
+  </si>
+  <si>
+    <t>Génération des réponses du chatbot (RAG) et appels aux modèles de langage</t>
+  </si>
+  <si>
+    <t>~5 000 requêtes/mois, ~1 000 tokens par requête</t>
+  </si>
+  <si>
+    <t>Trafic entrant/sortant, appels API externes (OpenAgenda, LLM)</t>
+  </si>
+  <si>
+    <t>Volumes faibles, inclus dans l’offre cloud</t>
+  </si>
+  <si>
+    <t>Collecte des métriques de performance, logs applicatifs, erreurs et supervision</t>
+  </si>
+  <si>
+    <t>Azure Monitor / Application Insights, faible volumétrie</t>
+  </si>
+  <si>
+    <t>Coût mensuel estimé</t>
+  </si>
+  <si>
+    <t>Inclus</t>
+  </si>
+  <si>
+    <t>Maintenance opérationnelle</t>
+  </si>
+  <si>
+    <t>Ajustements mineurs, surveillance, correctifs légers</t>
+  </si>
+  <si>
+    <t>Maintenance minimale en phase MVP</t>
+  </si>
+  <si>
+    <t>Critère</t>
+  </si>
+  <si>
+    <t>Microsoft Azure</t>
+  </si>
+  <si>
+    <t>Amazon Web Services</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform</t>
+  </si>
+  <si>
+    <t>Positionnement</t>
+  </si>
+  <si>
+    <t>Généraliste, orienté entreprise</t>
+  </si>
+  <si>
+    <t>Très large, très granulaire</t>
+  </si>
+  <si>
+    <t>Data &amp; ML centric</t>
+  </si>
+  <si>
+    <t>Simplicité de mise en œuvre (MVP)</t>
+  </si>
+  <si>
+    <t>Moyenne à faible</t>
+  </si>
+  <si>
+    <t>Services managés conteneurs</t>
+  </si>
+  <si>
+    <t>App Service / Container Apps simples</t>
+  </si>
+  <si>
+    <t>ECS / EKS plus complexes</t>
+  </si>
+  <si>
+    <t>Cloud Run efficace</t>
+  </si>
+  <si>
+    <t>Observabilité native</t>
+  </si>
+  <si>
+    <t>Azure Monitor intégré</t>
+  </si>
+  <si>
+    <t>CloudWatch à configurer</t>
+  </si>
+  <si>
+    <t>Cloud Monitoring</t>
+  </si>
+  <si>
+    <t>Lisibilité des coûts (faible charge)</t>
+  </si>
+  <si>
+    <t>Bonne</t>
+  </si>
+  <si>
+    <t>Plus complexe</t>
+  </si>
+  <si>
+    <t>Correcte</t>
+  </si>
+  <si>
+    <t>Adaptation à une démarche MVP</t>
+  </si>
+  <si>
+    <t>Très bonne</t>
+  </si>
+  <si>
+    <t>Scalabilité long terme</t>
+  </si>
+  <si>
+    <t>Très élevée</t>
+  </si>
+  <si>
+    <t>Temps de delivery</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>Plus long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -466,11 +590,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -512,6 +639,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -537,6 +680,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -634,49 +782,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8331DBB-6E1E-4B85-8785-A55B8CC33F84}" name="Tableau3" displayName="Tableau3" ref="A1:G13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8331DBB-6E1E-4B85-8785-A55B8CC33F84}" name="Tableau3" displayName="Tableau3" ref="A1:G13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:G13" xr:uid="{A8331DBB-6E1E-4B85-8785-A55B8CC33F84}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B253102F-999D-49F2-8E18-6693D9800FAF}" name="Fonctionnalité" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{091694F9-B98A-4B30-B710-F9D4188B797A}" name="Description" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{69D88119-F382-41A4-886C-742E3EFE38F2}" name="Priorité" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{BC292F91-34EA-48AD-BEC8-37943EAA4BC9}" name="Complexité" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{6A5A6642-FBC4-469C-898A-400513D58B4A}" name="Estimation délai" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{6203D995-4075-4C9A-A9B0-D9FF081DB35B}" name="Risques identifiés" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{3A88F841-B3F3-49BA-BB93-35C15A22BD3B}" name="Mitigation" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{B253102F-999D-49F2-8E18-6693D9800FAF}" name="Fonctionnalité" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{091694F9-B98A-4B30-B710-F9D4188B797A}" name="Description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{69D88119-F382-41A4-886C-742E3EFE38F2}" name="Priorité" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{BC292F91-34EA-48AD-BEC8-37943EAA4BC9}" name="Complexité" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{6A5A6642-FBC4-469C-898A-400513D58B4A}" name="Estimation délai" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{6203D995-4075-4C9A-A9B0-D9FF081DB35B}" name="Risques identifiés" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{3A88F841-B3F3-49BA-BB93-35C15A22BD3B}" name="Mitigation" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D8498DB-8A5E-4007-8CB5-AFD8FCACA27F}" name="Tableau2" displayName="Tableau2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:E11" xr:uid="{5D8498DB-8A5E-4007-8CB5-AFD8FCACA27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D8498DB-8A5E-4007-8CB5-AFD8FCACA27F}" name="Tableau2" displayName="Tableau2" ref="A1:E12" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:E12" xr:uid="{5D8498DB-8A5E-4007-8CB5-AFD8FCACA27F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F7536038-BADB-4908-9CE0-78C7BBE626F6}" name="Poste de coût" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{14198959-6421-47E2-AFA3-900AB15FD10C}" name="Description" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{D9CB58FA-66AB-4981-9C3A-4C3758DB890A}" name="Nature du coût" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6A8E4B49-EE11-490A-97B0-6963D6BAD4B5}" name="Complexité" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{7CF99FD3-EE24-4A55-95F6-11DD0FD1FD96}" name="Charge estimée" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{F7536038-BADB-4908-9CE0-78C7BBE626F6}" name="Poste de coût" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{14198959-6421-47E2-AFA3-900AB15FD10C}" name="Description" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{D9CB58FA-66AB-4981-9C3A-4C3758DB890A}" name="Nature du coût" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{6A8E4B49-EE11-490A-97B0-6963D6BAD4B5}" name="Charge estimée" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{7CF99FD3-EE24-4A55-95F6-11DD0FD1FD96}" name="Coût" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6487FF63-79C1-4C76-83F3-D7D984B69CE9}" name="Tableau1" displayName="Tableau1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:D8" xr:uid="{6487FF63-79C1-4C76-83F3-D7D984B69CE9}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{82A3D2B7-575C-4B93-B2B7-B6E9BBC4155F}" name="Poste de coût" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1E6B3D92-27B9-411F-BCD1-1AD3124A4351}" name="Description" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CB008C46-A766-4832-AE8F-F79DD1BCF76F}" name="Type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{A55A3BFA-73DE-4F95-99F7-9963B1467CAE}" name="Impact selon charge utilisateur" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6487FF63-79C1-4C76-83F3-D7D984B69CE9}" name="Tableau1" displayName="Tableau1" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9" xr:uid="{6487FF63-79C1-4C76-83F3-D7D984B69CE9}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{82A3D2B7-575C-4B93-B2B7-B6E9BBC4155F}" name="Poste de coût"/>
+    <tableColumn id="2" xr3:uid="{1E6B3D92-27B9-411F-BCD1-1AD3124A4351}" name="Détail du périmètre couvert"/>
+    <tableColumn id="3" xr3:uid="{CB008C46-A766-4832-AE8F-F79DD1BCF76F}" name="Hypothèses retenues"/>
+    <tableColumn id="4" xr3:uid="{A55A3BFA-73DE-4F95-99F7-9963B1467CAE}" name="Type de coût"/>
+    <tableColumn id="5" xr3:uid="{5BA19FC7-76CA-42EA-B991-017743AB501C}" name="Coût mensuel estimé" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3ECB7ABC-F674-49C0-AFA0-A846DF389433}" name="Tableau5" displayName="Tableau5" ref="A1:D9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:D9" xr:uid="{3ECB7ABC-F674-49C0-AFA0-A846DF389433}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4027E3D7-97F8-4858-B50A-0C16CB1DCF00}" name="Critère" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D169F9FE-EA67-4F6D-9AA8-EEDE3B8C448B}" name="Microsoft Azure" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4E4A6A9C-7E64-48A7-AD0D-5C538AFB030D}" name="Amazon Web Services" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{BA85CD0B-1D73-4736-9CBD-9604363EDAE6}" name="Google Cloud Platform" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5FD850C7-DAAD-4333-9D96-5E598DA30E86}" name="Tableau4" displayName="Tableau4" ref="A1:C7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C7" xr:uid="{5FD850C7-DAAD-4333-9D96-5E598DA30E86}"/>
   <tableColumns count="3">
@@ -1278,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A30E42-E070-4008-B90E-CCE07BAD58AB}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1304,10 +1466,10 @@
         <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -1321,10 +1483,10 @@
         <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1338,10 +1500,10 @@
         <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2500</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -1355,27 +1517,27 @@
         <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1383,16 +1545,16 @@
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1400,16 +1562,16 @@
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>116</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3000</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1417,67 +1579,80 @@
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2500</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="4">
+        <v>16500</v>
       </c>
     </row>
   </sheetData>
@@ -1490,129 +1665,314 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63C18F6-3084-40DB-AF2E-D4A3C5D32FEF}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="E2" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="4">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6155F561-938E-4CD4-8B21-8FD19CABE254}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1623,11 +1983,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795ED52E-C796-48C8-A3C9-C0F85C7811EC}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1640,68 +2000,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -1709,10 +2069,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>